<commit_message>
Processed R451645.pdf → 20260212_d3c70a24-378f-42e1-b71c-9767071cea25
</commit_message>
<xml_diff>
--- a/data/documents.xlsx
+++ b/data/documents.xlsx
@@ -491,8 +491,16 @@
           <t>False</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20260212_d3c70a24-378f-42e1-b71c-9767071cea25</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>submitted</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Processed R451644.pdf → 20260212_25e4fbdf-503a-4175-9c26-217e2f99368a
</commit_message>
<xml_diff>
--- a/data/documents.xlsx
+++ b/data/documents.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20260212_2c7ea7da-a9ce-4a73-8b37-d5bfc41296ef</t>
+          <t>20260212_25e4fbdf-503a-4175-9c26-217e2f99368a</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Processed R451645.pdf → 20260212_9b0d0d82-9c28-46d1-8de3-67fb2141469e
</commit_message>
<xml_diff>
--- a/data/documents.xlsx
+++ b/data/documents.xlsx
@@ -488,12 +488,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20260212_4d83ce4a-e8f1-4d67-b125-c9723d5f2ca0</t>
+          <t>20260212_9b0d0d82-9c28-46d1-8de3-67fb2141469e</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>